<commit_message>
Enhanced Task 3 with updating results
</commit_message>
<xml_diff>
--- a/Test Form.xlsx
+++ b/Test Form.xlsx
@@ -78,7 +78,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -92,6 +92,9 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -100,6 +103,9 @@
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,7 +472,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,15 +480,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="6" width="13.14785714285714"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="6" width="22.14785714285714"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="7" width="16.43357142857143"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="6" width="9.005000000000001"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="7" width="21.14785714285714"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="6" width="23.71928571428571"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="6" width="12.005"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="6" width="24.57642857142857"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="6" width="21.29071428571428"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="7" width="13.14785714285714"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="7" width="22.14785714285714"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="8" width="16.43357142857143"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="7" width="9.005000000000001"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="8" width="21.14785714285714"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="7" width="23.71928571428571"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="7" width="12.005"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="7" width="24.57642857142857"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" style="9" width="21.14785714285714"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="7" width="21.29071428571428"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="18.75" r="1">
@@ -531,6 +538,11 @@
           <t>Expected Behaviour</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Actual Behaviour</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -570,6 +582,11 @@
           <t>Should Pass</t>
         </is>
       </c>
+      <c r="J2" s="5" t="inlineStr">
+        <is>
+          <t>Passed as expected</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -609,6 +626,11 @@
           <t>Should Fail</t>
         </is>
       </c>
+      <c r="J3" s="5" t="inlineStr">
+        <is>
+          <t>Failed as expected</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="19.5" r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -616,7 +638,7 @@
           <t>Sneha Iyer</t>
         </is>
       </c>
-      <c r="B4" s="5" t="n"/>
+      <c r="B4" s="6" t="n"/>
       <c r="C4" s="4" t="n">
         <v>9821345678</v>
       </c>
@@ -648,6 +670,11 @@
           <t>Should Fail</t>
         </is>
       </c>
+      <c r="J4" s="5" t="inlineStr">
+        <is>
+          <t>Failed as expected</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -685,6 +712,11 @@
       <c r="I5" s="3" t="inlineStr">
         <is>
           <t>Should Pass</t>
+        </is>
+      </c>
+      <c r="J5" s="5" t="inlineStr">
+        <is>
+          <t>Passed as expected</t>
         </is>
       </c>
     </row>
@@ -722,6 +754,11 @@
           <t>Should Fail</t>
         </is>
       </c>
+      <c r="J6" s="5" t="inlineStr">
+        <is>
+          <t>Failed as expected</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -765,6 +802,11 @@
           <t>Should Pass</t>
         </is>
       </c>
+      <c r="J7" s="5" t="inlineStr">
+        <is>
+          <t>Passed as expected</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="19.5" r="8">
       <c r="A8" s="3" t="inlineStr">
@@ -772,7 +814,7 @@
           <t>Kavya Rao</t>
         </is>
       </c>
-      <c r="B8" s="5" t="inlineStr">
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>kavya.raogmail.com</t>
         </is>
@@ -804,6 +846,11 @@
           <t>Should Fail</t>
         </is>
       </c>
+      <c r="J8" s="5" t="inlineStr">
+        <is>
+          <t>Failed as expected</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="9">
       <c r="A9" s="3" t="inlineStr">
@@ -847,6 +894,11 @@
           <t>Should Pass</t>
         </is>
       </c>
+      <c r="J9" s="5" t="inlineStr">
+        <is>
+          <t>Passed as expected</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="10">
       <c r="A10" s="3" t="inlineStr">
@@ -884,6 +936,11 @@
       <c r="I10" s="3" t="inlineStr">
         <is>
           <t>Should Fail</t>
+        </is>
+      </c>
+      <c r="J10" s="5" t="inlineStr">
+        <is>
+          <t>Failed as expected</t>
         </is>
       </c>
     </row>
@@ -919,6 +976,11 @@
       <c r="I11" s="3" t="inlineStr">
         <is>
           <t>Should Fail</t>
+        </is>
+      </c>
+      <c r="J11" s="5" t="inlineStr">
+        <is>
+          <t>Failed as expected</t>
         </is>
       </c>
     </row>

</xml_diff>